<commit_message>
add medical and traffice score
</commit_message>
<xml_diff>
--- a/指标.xlsx
+++ b/指标.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>教育得分</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>教育</t>
+  </si>
+  <si>
+    <t>交通</t>
+  </si>
+  <si>
+    <t>医疗</t>
+  </si>
+  <si>
+    <t>得分</t>
   </si>
   <si>
     <t>上海市</t>
@@ -455,231 +464,483 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>5.2</v>
+      </c>
+      <c r="D2">
+        <v>5.2</v>
+      </c>
+      <c r="E2">
+        <v>5.733333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>3.4</v>
+      </c>
+      <c r="D3">
+        <v>3.4</v>
+      </c>
+      <c r="E3">
+        <v>3.933333333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>2.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>3.8</v>
+      </c>
+      <c r="D4">
+        <v>3.8</v>
+      </c>
+      <c r="E4">
+        <v>3.299999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>3.6</v>
+      </c>
+      <c r="D5">
+        <v>3.6</v>
+      </c>
+      <c r="E5">
+        <v>3.166666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>6.2</v>
+      </c>
+      <c r="D6">
+        <v>6.2</v>
+      </c>
+      <c r="E6">
+        <v>5.533333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>4.4</v>
+      </c>
+      <c r="D7">
+        <v>4.4</v>
+      </c>
+      <c r="E7">
+        <v>4.100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>4.3</v>
+      </c>
+      <c r="D8">
+        <v>4.3</v>
+      </c>
+      <c r="E8">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1.366666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>1.1</v>
+      </c>
+      <c r="D10">
+        <v>1.1</v>
+      </c>
+      <c r="E10">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>4.2</v>
+      </c>
+      <c r="D11">
+        <v>4.2</v>
+      </c>
+      <c r="E11">
+        <v>4.566666666666666</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>3.5</v>
+      </c>
+      <c r="D12">
+        <v>3.5</v>
+      </c>
+      <c r="E12">
+        <v>3.466666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>4.1</v>
+      </c>
+      <c r="D13">
+        <v>4.1</v>
+      </c>
+      <c r="E13">
+        <v>3.533333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>2.4</v>
+      </c>
+      <c r="D14">
+        <v>2.4</v>
+      </c>
+      <c r="E14">
+        <v>2.533333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>3.6</v>
+      </c>
+      <c r="D15">
+        <v>3.6</v>
+      </c>
+      <c r="E15">
+        <v>3.066666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>2.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>3.433333333333334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3.033333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>2.6</v>
+      </c>
+      <c r="D18">
+        <v>2.6</v>
+      </c>
+      <c r="E18">
+        <v>2.633333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>3.3</v>
+      </c>
+      <c r="D19">
+        <v>3.3</v>
+      </c>
+      <c r="E19">
+        <v>3.366666666666667</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>3.5</v>
+      </c>
+      <c r="D20">
+        <v>3.5</v>
+      </c>
+      <c r="E20">
+        <v>2.866666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>1.3</v>
+      </c>
+      <c r="D21">
+        <v>1.3</v>
+      </c>
+      <c r="E21">
+        <v>1.933333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>2.2</v>
+      </c>
+      <c r="D22">
+        <v>2.2</v>
+      </c>
+      <c r="E22">
+        <v>2.533333333333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>4.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>1.6</v>
+      </c>
+      <c r="D23">
+        <v>1.6</v>
+      </c>
+      <c r="E23">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>1.8</v>
+      </c>
+      <c r="D24">
+        <v>1.8</v>
+      </c>
+      <c r="E24">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>3.7</v>
+      </c>
+      <c r="D25">
+        <v>3.7</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>0.9</v>
+      </c>
+      <c r="D26">
+        <v>0.9</v>
+      </c>
+      <c r="E26">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>5.4</v>
+      </c>
+      <c r="D27">
+        <v>5.4</v>
+      </c>
+      <c r="E27">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>4.4</v>
+      </c>
+      <c r="C28">
+        <v>4.1</v>
+      </c>
+      <c r="D28">
+        <v>4.1</v>
+      </c>
+      <c r="E28">
+        <v>4.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add medical and traffiic score
</commit_message>
<xml_diff>
--- a/指标.xlsx
+++ b/指标.xlsx
@@ -25,88 +25,88 @@
     <t>医疗</t>
   </si>
   <si>
-    <t>得分</t>
+    <t>平均分</t>
   </si>
   <si>
     <t>上海市</t>
   </si>
   <si>
+    <t>池州市</t>
+  </si>
+  <si>
+    <t>舟山市</t>
+  </si>
+  <si>
+    <t>南京市</t>
+  </si>
+  <si>
+    <t>芜湖市</t>
+  </si>
+  <si>
+    <t>金华市</t>
+  </si>
+  <si>
+    <t>滁州市</t>
+  </si>
+  <si>
     <t>合肥市</t>
   </si>
   <si>
+    <t>常州市</t>
+  </si>
+  <si>
+    <t>南通市</t>
+  </si>
+  <si>
+    <t>泰州市</t>
+  </si>
+  <si>
+    <t>镇江市</t>
+  </si>
+  <si>
     <t>安庆市</t>
   </si>
   <si>
     <t>宣城市</t>
   </si>
   <si>
-    <t>池州市</t>
-  </si>
-  <si>
-    <t>滁州市</t>
-  </si>
-  <si>
-    <t>芜湖市</t>
+    <t>无锡市</t>
+  </si>
+  <si>
+    <t>盐城市</t>
+  </si>
+  <si>
+    <t>湖州市</t>
+  </si>
+  <si>
+    <t>台州市</t>
+  </si>
+  <si>
+    <t>杭州市</t>
+  </si>
+  <si>
+    <t>苏州市</t>
+  </si>
+  <si>
+    <t>宁波市</t>
+  </si>
+  <si>
+    <t>扬州市</t>
+  </si>
+  <si>
+    <t>温州市</t>
+  </si>
+  <si>
+    <t>嘉兴市</t>
+  </si>
+  <si>
+    <t>绍兴市</t>
+  </si>
+  <si>
+    <t>马鞍山市</t>
   </si>
   <si>
     <t>铜陵市</t>
-  </si>
-  <si>
-    <t>马鞍山市</t>
-  </si>
-  <si>
-    <t>南京市</t>
-  </si>
-  <si>
-    <t>南通市</t>
-  </si>
-  <si>
-    <t>常州市</t>
-  </si>
-  <si>
-    <t>扬州市</t>
-  </si>
-  <si>
-    <t>无锡市</t>
-  </si>
-  <si>
-    <t>泰州市</t>
-  </si>
-  <si>
-    <t>盐城市</t>
-  </si>
-  <si>
-    <t>苏州市</t>
-  </si>
-  <si>
-    <t>镇江市</t>
-  </si>
-  <si>
-    <t>台州市</t>
-  </si>
-  <si>
-    <t>嘉兴市</t>
-  </si>
-  <si>
-    <t>宁波市</t>
-  </si>
-  <si>
-    <t>杭州市</t>
-  </si>
-  <si>
-    <t>温州市</t>
-  </si>
-  <si>
-    <t>湖州市</t>
-  </si>
-  <si>
-    <t>绍兴市</t>
-  </si>
-  <si>
-    <t>舟山市</t>
-  </si>
-  <si>
-    <t>金华市</t>
   </si>
 </sst>
 </file>
@@ -506,16 +506,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="C3">
-        <v>3.4</v>
+        <v>6.2</v>
       </c>
       <c r="D3">
-        <v>3.4</v>
+        <v>6.2</v>
       </c>
       <c r="E3">
-        <v>3.933333333333334</v>
+        <v>5.533333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -523,16 +523,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2.3</v>
+        <v>3.3</v>
       </c>
       <c r="C4">
-        <v>3.8</v>
+        <v>5.4</v>
       </c>
       <c r="D4">
-        <v>3.8</v>
+        <v>5.4</v>
       </c>
       <c r="E4">
-        <v>3.299999999999999</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -540,16 +540,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>2.3</v>
+        <v>5.3</v>
       </c>
       <c r="C5">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="D5">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="E5">
-        <v>3.166666666666667</v>
+        <v>4.566666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -557,16 +557,16 @@
         <v>8</v>
       </c>
       <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4.3</v>
+      </c>
+      <c r="D6">
+        <v>4.3</v>
+      </c>
+      <c r="E6">
         <v>4.2</v>
-      </c>
-      <c r="C6">
-        <v>6.2</v>
-      </c>
-      <c r="D6">
-        <v>6.2</v>
-      </c>
-      <c r="E6">
-        <v>5.533333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -574,16 +574,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>3.5</v>
+        <v>4.4</v>
       </c>
       <c r="C7">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="D7">
-        <v>4.4</v>
+        <v>4.1</v>
       </c>
       <c r="E7">
-        <v>4.100000000000001</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -591,16 +591,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="C8">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="D8">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="E8">
-        <v>4.2</v>
+        <v>4.100000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -608,16 +608,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>2.1</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="E9">
-        <v>1.366666666666666</v>
+        <v>3.933333333333334</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -625,16 +625,16 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="C10">
-        <v>1.1</v>
+        <v>4.1</v>
       </c>
       <c r="D10">
-        <v>1.1</v>
+        <v>4.1</v>
       </c>
       <c r="E10">
-        <v>1.4</v>
+        <v>3.533333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -642,16 +642,16 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>5.3</v>
+        <v>3.4</v>
       </c>
       <c r="C11">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="D11">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E11">
-        <v>4.566666666666666</v>
+        <v>3.466666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -659,16 +659,16 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>3.4</v>
+        <v>2.3</v>
       </c>
       <c r="C12">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>3.466666666666667</v>
+        <v>3.433333333333334</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -676,16 +676,16 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>2.4</v>
+        <v>3.5</v>
       </c>
       <c r="C13">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="D13">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="E13">
-        <v>3.533333333333333</v>
+        <v>3.366666666666667</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -693,16 +693,16 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>2.8</v>
+        <v>2.3</v>
       </c>
       <c r="C14">
-        <v>2.4</v>
+        <v>3.8</v>
       </c>
       <c r="D14">
-        <v>2.4</v>
+        <v>3.8</v>
       </c>
       <c r="E14">
-        <v>2.533333333333333</v>
+        <v>3.299999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -710,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>2.3</v>
       </c>
       <c r="C15">
         <v>3.6</v>
@@ -719,7 +719,7 @@
         <v>3.6</v>
       </c>
       <c r="E15">
-        <v>3.066666666666666</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -727,16 +727,16 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>2.3</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="E16">
-        <v>3.433333333333334</v>
+        <v>3.066666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -761,16 +761,16 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>2.7</v>
+        <v>1.6</v>
       </c>
       <c r="C18">
-        <v>2.6</v>
+        <v>3.7</v>
       </c>
       <c r="D18">
-        <v>2.6</v>
+        <v>3.7</v>
       </c>
       <c r="E18">
-        <v>2.633333333333333</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -778,16 +778,16 @@
         <v>21</v>
       </c>
       <c r="B19">
+        <v>1.6</v>
+      </c>
+      <c r="C19">
         <v>3.5</v>
       </c>
-      <c r="C19">
-        <v>3.3</v>
-      </c>
       <c r="D19">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="E19">
-        <v>3.366666666666667</v>
+        <v>2.866666666666667</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -795,16 +795,16 @@
         <v>22</v>
       </c>
       <c r="B20">
+        <v>4.9</v>
+      </c>
+      <c r="C20">
         <v>1.6</v>
       </c>
-      <c r="C20">
-        <v>3.5</v>
-      </c>
       <c r="D20">
-        <v>3.5</v>
+        <v>1.6</v>
       </c>
       <c r="E20">
-        <v>2.866666666666667</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -812,16 +812,16 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="C21">
-        <v>1.3</v>
+        <v>2.6</v>
       </c>
       <c r="D21">
-        <v>1.3</v>
+        <v>2.6</v>
       </c>
       <c r="E21">
-        <v>1.933333333333333</v>
+        <v>2.633333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -846,16 +846,16 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>4.9</v>
+        <v>2.8</v>
       </c>
       <c r="C23">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="D23">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="E23">
-        <v>2.7</v>
+        <v>2.533333333333333</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -880,16 +880,16 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="C25">
-        <v>3.7</v>
+        <v>1.3</v>
       </c>
       <c r="D25">
-        <v>3.7</v>
+        <v>1.3</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>1.933333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -914,16 +914,16 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>3.3</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>5.4</v>
+        <v>1.1</v>
       </c>
       <c r="D27">
-        <v>5.4</v>
+        <v>1.1</v>
       </c>
       <c r="E27">
-        <v>4.7</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -931,16 +931,16 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>4.4</v>
+        <v>2.1</v>
       </c>
       <c r="C28">
-        <v>4.1</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>4.1</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>4.2</v>
+        <v>1.366666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>